<commit_message>
Rename columns in data files
</commit_message>
<xml_diff>
--- a/data/Airlines.xlsx
+++ b/data/Airlines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krzysiek\Documents\GitHub\flight_db\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9AA5F0-E2F1-43B2-A37A-59B59101BA9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D578F1-5EC8-494D-BF05-C2DF2B384E5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{215C9B6B-8696-49E5-8EBC-05913498BF43}"/>
   </bookViews>
@@ -36,12 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
-    <t>AirlineId</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Ryanair</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
     <t>Air Canada</t>
   </si>
   <si>
-    <t>AirlineCode</t>
-  </si>
-  <si>
     <t>RYR</t>
   </si>
   <si>
@@ -109,6 +100,15 @@
   </si>
   <si>
     <t>LOT</t>
+  </si>
+  <si>
+    <t>airline_id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>airline_code</t>
   </si>
 </sst>
 </file>
@@ -473,20 +473,20 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -494,10 +494,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -505,10 +505,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -516,10 +516,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -527,10 +527,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -538,10 +538,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -549,10 +549,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -560,10 +560,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -571,10 +571,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -582,10 +582,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -593,10 +593,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -604,10 +604,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>